<commit_message>
Fix Data Column Names
</commit_message>
<xml_diff>
--- a/Data/Census Data and Data_Of_Interest.xlsx
+++ b/Data/Census Data and Data_Of_Interest.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melekmizher/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melekmizher/Documents/GitHub/Mizher_MSDS455_Assignment2_CategoricalData/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25EF230C-4B88-3A4E-8C32-CAE4DADAD0E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA207951-ADDC-6341-868D-8AAD354A1B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="76800" windowHeight="43200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="76800" windowHeight="40040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="130">
   <si>
     <t>Table with row headers in column A and column headers in rows 7 through 8</t>
   </si>
@@ -1130,6 +1130,21 @@
   <si>
     <t>Not a citizen</t>
   </si>
+  <si>
+    <t>Total_Population</t>
+  </si>
+  <si>
+    <t>Any_Insured</t>
+  </si>
+  <si>
+    <t>Private_Insured</t>
+  </si>
+  <si>
+    <t>Public_Insured</t>
+  </si>
+  <si>
+    <t>Uninsured</t>
+  </si>
 </sst>
 </file>
 
@@ -1138,9 +1153,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="##0.0"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1234,6 +1256,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1321,50 +1349,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1717,172 +1749,172 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
     </row>
     <row r="2" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11" t="s">
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11" t="s">
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11" t="s">
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
     </row>
     <row r="8" spans="1:18" ht="27" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
@@ -6139,117 +6171,139 @@
       </c>
     </row>
     <row r="92" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="9" t="s">
+      <c r="A92" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="B92" s="9"/>
-      <c r="C92" s="9"/>
-      <c r="D92" s="9"/>
-      <c r="E92" s="9"/>
-      <c r="F92" s="9"/>
-      <c r="G92" s="9"/>
-      <c r="H92" s="9"/>
-      <c r="I92" s="9"/>
-      <c r="J92" s="9"/>
-      <c r="K92" s="9"/>
-      <c r="L92" s="9"/>
-      <c r="M92" s="9"/>
-      <c r="N92" s="9"/>
-      <c r="O92" s="9"/>
-      <c r="P92" s="9"/>
-      <c r="Q92" s="9"/>
-      <c r="R92" s="9"/>
+      <c r="B92" s="13"/>
+      <c r="C92" s="13"/>
+      <c r="D92" s="13"/>
+      <c r="E92" s="13"/>
+      <c r="F92" s="13"/>
+      <c r="G92" s="13"/>
+      <c r="H92" s="13"/>
+      <c r="I92" s="13"/>
+      <c r="J92" s="13"/>
+      <c r="K92" s="13"/>
+      <c r="L92" s="13"/>
+      <c r="M92" s="13"/>
+      <c r="N92" s="13"/>
+      <c r="O92" s="13"/>
+      <c r="P92" s="13"/>
+      <c r="Q92" s="13"/>
+      <c r="R92" s="13"/>
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A93" s="8" t="s">
+      <c r="A93" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="B93" s="8"/>
-      <c r="C93" s="8"/>
-      <c r="D93" s="8"/>
-      <c r="E93" s="8"/>
-      <c r="F93" s="8"/>
-      <c r="G93" s="8"/>
-      <c r="H93" s="8"/>
-      <c r="I93" s="8"/>
-      <c r="J93" s="8"/>
-      <c r="K93" s="8"/>
-      <c r="L93" s="8"/>
-      <c r="M93" s="8"/>
-      <c r="N93" s="8"/>
-      <c r="O93" s="8"/>
-      <c r="P93" s="8"/>
-      <c r="Q93" s="8"/>
-      <c r="R93" s="8"/>
+      <c r="B93" s="11"/>
+      <c r="C93" s="11"/>
+      <c r="D93" s="11"/>
+      <c r="E93" s="11"/>
+      <c r="F93" s="11"/>
+      <c r="G93" s="11"/>
+      <c r="H93" s="11"/>
+      <c r="I93" s="11"/>
+      <c r="J93" s="11"/>
+      <c r="K93" s="11"/>
+      <c r="L93" s="11"/>
+      <c r="M93" s="11"/>
+      <c r="N93" s="11"/>
+      <c r="O93" s="11"/>
+      <c r="P93" s="11"/>
+      <c r="Q93" s="11"/>
+      <c r="R93" s="11"/>
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A94" s="8" t="s">
+      <c r="A94" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B94" s="8"/>
-      <c r="C94" s="8"/>
-      <c r="D94" s="8"/>
-      <c r="E94" s="8"/>
-      <c r="F94" s="8"/>
-      <c r="G94" s="8"/>
-      <c r="H94" s="8"/>
-      <c r="I94" s="8"/>
-      <c r="J94" s="8"/>
-      <c r="K94" s="8"/>
-      <c r="L94" s="8"/>
-      <c r="M94" s="8"/>
-      <c r="N94" s="8"/>
-      <c r="O94" s="8"/>
-      <c r="P94" s="8"/>
-      <c r="Q94" s="8"/>
-      <c r="R94" s="8"/>
+      <c r="B94" s="11"/>
+      <c r="C94" s="11"/>
+      <c r="D94" s="11"/>
+      <c r="E94" s="11"/>
+      <c r="F94" s="11"/>
+      <c r="G94" s="11"/>
+      <c r="H94" s="11"/>
+      <c r="I94" s="11"/>
+      <c r="J94" s="11"/>
+      <c r="K94" s="11"/>
+      <c r="L94" s="11"/>
+      <c r="M94" s="11"/>
+      <c r="N94" s="11"/>
+      <c r="O94" s="11"/>
+      <c r="P94" s="11"/>
+      <c r="Q94" s="11"/>
+      <c r="R94" s="11"/>
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A95" s="8" t="s">
+      <c r="A95" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B95" s="8"/>
-      <c r="C95" s="8"/>
-      <c r="D95" s="8"/>
-      <c r="E95" s="8"/>
-      <c r="F95" s="8"/>
-      <c r="G95" s="8"/>
-      <c r="H95" s="8"/>
-      <c r="I95" s="8"/>
-      <c r="J95" s="8"/>
-      <c r="K95" s="8"/>
-      <c r="L95" s="8"/>
-      <c r="M95" s="8"/>
-      <c r="N95" s="8"/>
-      <c r="O95" s="8"/>
-      <c r="P95" s="8"/>
-      <c r="Q95" s="8"/>
-      <c r="R95" s="8"/>
+      <c r="B95" s="11"/>
+      <c r="C95" s="11"/>
+      <c r="D95" s="11"/>
+      <c r="E95" s="11"/>
+      <c r="F95" s="11"/>
+      <c r="G95" s="11"/>
+      <c r="H95" s="11"/>
+      <c r="I95" s="11"/>
+      <c r="J95" s="11"/>
+      <c r="K95" s="11"/>
+      <c r="L95" s="11"/>
+      <c r="M95" s="11"/>
+      <c r="N95" s="11"/>
+      <c r="O95" s="11"/>
+      <c r="P95" s="11"/>
+      <c r="Q95" s="11"/>
+      <c r="R95" s="11"/>
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A96" s="8" t="s">
+      <c r="A96" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="B96" s="8"/>
-      <c r="C96" s="8"/>
-      <c r="D96" s="8"/>
-      <c r="E96" s="8"/>
-      <c r="F96" s="8"/>
-      <c r="G96" s="8"/>
-      <c r="H96" s="8"/>
-      <c r="I96" s="8"/>
-      <c r="J96" s="8"/>
-      <c r="K96" s="8"/>
-      <c r="L96" s="8"/>
-      <c r="M96" s="8"/>
-      <c r="N96" s="8"/>
-      <c r="O96" s="8"/>
-      <c r="P96" s="8"/>
-      <c r="Q96" s="8"/>
-      <c r="R96" s="8"/>
+      <c r="B96" s="11"/>
+      <c r="C96" s="11"/>
+      <c r="D96" s="11"/>
+      <c r="E96" s="11"/>
+      <c r="F96" s="11"/>
+      <c r="G96" s="11"/>
+      <c r="H96" s="11"/>
+      <c r="I96" s="11"/>
+      <c r="J96" s="11"/>
+      <c r="K96" s="11"/>
+      <c r="L96" s="11"/>
+      <c r="M96" s="11"/>
+      <c r="N96" s="11"/>
+      <c r="O96" s="11"/>
+      <c r="P96" s="11"/>
+      <c r="Q96" s="11"/>
+      <c r="R96" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="A3:R3"/>
+    <mergeCell ref="A4:R4"/>
+    <mergeCell ref="A5:R5"/>
+    <mergeCell ref="A6:R6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="O7:R7"/>
+    <mergeCell ref="A10:R10"/>
+    <mergeCell ref="A17:R17"/>
+    <mergeCell ref="A26:R26"/>
+    <mergeCell ref="A29:R29"/>
+    <mergeCell ref="A34:R34"/>
+    <mergeCell ref="A39:R39"/>
+    <mergeCell ref="A47:R47"/>
+    <mergeCell ref="A53:R53"/>
+    <mergeCell ref="A57:R57"/>
+    <mergeCell ref="A65:R65"/>
     <mergeCell ref="A94:R94"/>
     <mergeCell ref="A95:R95"/>
     <mergeCell ref="A96:R96"/>
@@ -6258,28 +6312,6 @@
     <mergeCell ref="A85:R85"/>
     <mergeCell ref="A92:R92"/>
     <mergeCell ref="A93:R93"/>
-    <mergeCell ref="A39:R39"/>
-    <mergeCell ref="A47:R47"/>
-    <mergeCell ref="A53:R53"/>
-    <mergeCell ref="A57:R57"/>
-    <mergeCell ref="A65:R65"/>
-    <mergeCell ref="A10:R10"/>
-    <mergeCell ref="A17:R17"/>
-    <mergeCell ref="A26:R26"/>
-    <mergeCell ref="A29:R29"/>
-    <mergeCell ref="A34:R34"/>
-    <mergeCell ref="A6:R6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="O7:R7"/>
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="A2:R2"/>
-    <mergeCell ref="A3:R3"/>
-    <mergeCell ref="A4:R4"/>
-    <mergeCell ref="A5:R5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -6300,1422 +6332,1422 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" ht="52" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="6" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="10">
         <v>328074</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="10">
         <v>300887</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="10">
         <v>216366</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="10">
         <v>117095</v>
       </c>
-      <c r="F2" s="17">
+      <c r="F2" s="10">
         <v>27187</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="10">
         <v>263127</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="10">
         <v>242912</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="10">
         <v>177408</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="10">
         <v>90310</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="10">
         <v>20214</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="10">
         <v>84283</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="10">
         <v>78097</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="10">
         <v>59746</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="10">
         <v>29890</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="10">
         <v>6187</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="10">
         <v>71491</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="10">
         <v>68047</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="10">
         <v>44478</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="10">
         <v>25905</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="10">
         <v>3444</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="10">
         <v>21566</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="10">
         <v>20510</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="10">
         <v>13017</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="10">
         <v>8206</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="10">
         <v>1055</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="10">
         <v>1024</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="10">
         <v>864</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="10">
         <v>474</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="10">
         <v>416</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="10">
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="10">
         <v>63923</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="10">
         <v>57111</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="10">
         <v>38483</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="10">
         <v>26369</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="10">
         <v>6812</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="10">
         <v>271881</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="10">
         <v>245349</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="10">
         <v>188988</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="10">
         <v>64536</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="10">
         <v>26532</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="27" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="10">
         <v>77026</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="10">
         <v>73140</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="10">
         <v>47643</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="10">
         <v>28053</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="10">
         <v>3886</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="10">
         <v>194855</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="10">
         <v>172209</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="10">
         <v>141344</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="10">
         <v>36483</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="10">
         <v>22646</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="10">
         <v>29045</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="10">
         <v>24726</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="10">
         <v>19812</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="10">
         <v>5582</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="10">
         <v>4318</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B13" s="17">
+      <c r="B13" s="10">
         <v>40312</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="10">
         <v>34886</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="10">
         <v>28447</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="10">
         <v>7592</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="10">
         <v>5426</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B14" s="17">
+      <c r="B14" s="10">
         <v>43190</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="10">
         <v>38036</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="10">
         <v>31767</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="10">
         <v>7559</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="10">
         <v>5154</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B15" s="17">
+      <c r="B15" s="10">
         <v>82308</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="10">
         <v>74560</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="10">
         <v>61318</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="10">
         <v>15749</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="10">
         <v>7748</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="17">
+      <c r="B16" s="10">
         <v>56193</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C16" s="10">
         <v>55538</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="10">
         <v>27378</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="10">
         <v>52559</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="10">
         <v>655</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="17">
+      <c r="B17" s="10">
         <v>161758</v>
       </c>
-      <c r="C17" s="17">
+      <c r="C17" s="10">
         <v>146604</v>
       </c>
-      <c r="D17" s="17">
+      <c r="D17" s="10">
         <v>107186</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="10">
         <v>54672</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="10">
         <v>15154</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="17">
+      <c r="B18" s="10">
         <v>166316</v>
       </c>
-      <c r="C18" s="17">
+      <c r="C18" s="10">
         <v>154283</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="10">
         <v>109179</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="10">
         <v>62422</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="10">
         <v>12033</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="17">
+      <c r="B19" s="10">
         <v>281229</v>
       </c>
-      <c r="C19" s="17">
+      <c r="C19" s="10">
         <v>263172</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="10">
         <v>190775</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="10">
         <v>102229</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="10">
         <v>18057</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="17">
+      <c r="B20" s="10">
         <v>46845</v>
       </c>
-      <c r="C20" s="17">
+      <c r="C20" s="10">
         <v>37715</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="10">
         <v>25591</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="10">
         <v>14865</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="10">
         <v>9130</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B21" s="17">
+      <c r="B21" s="10">
         <v>22877</v>
       </c>
-      <c r="C21" s="17">
+      <c r="C21" s="10">
         <v>21078</v>
       </c>
-      <c r="D21" s="17">
+      <c r="D21" s="10">
         <v>14301</v>
       </c>
-      <c r="E21" s="17">
+      <c r="E21" s="10">
         <v>8863</v>
       </c>
-      <c r="F21" s="17">
+      <c r="F21" s="10">
         <v>1799</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B22" s="17">
+      <c r="B22" s="10">
         <v>23968</v>
       </c>
-      <c r="C22" s="17">
+      <c r="C22" s="10">
         <v>16637</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="10">
         <v>11290</v>
       </c>
-      <c r="E22" s="17">
+      <c r="E22" s="10">
         <v>6003</v>
       </c>
-      <c r="F22" s="17">
+      <c r="F22" s="10">
         <v>7331</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="17">
+      <c r="B23" s="10">
         <v>56065</v>
       </c>
-      <c r="C23" s="17">
+      <c r="C23" s="10">
         <v>53111</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="10">
         <v>38153</v>
       </c>
-      <c r="E23" s="17">
+      <c r="E23" s="10">
         <v>21755</v>
       </c>
-      <c r="F23" s="17">
+      <c r="F23" s="10">
         <v>2954</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="17">
+      <c r="B24" s="10">
         <v>67933</v>
       </c>
-      <c r="C24" s="17">
+      <c r="C24" s="10">
         <v>64170</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="10">
         <v>48222</v>
       </c>
-      <c r="E24" s="17">
+      <c r="E24" s="10">
         <v>23990</v>
       </c>
-      <c r="F24" s="17">
+      <c r="F24" s="10">
         <v>3762</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="17">
+      <c r="B25" s="10">
         <v>126144</v>
       </c>
-      <c r="C25" s="17">
+      <c r="C25" s="10">
         <v>111825</v>
       </c>
-      <c r="D25" s="17">
+      <c r="D25" s="10">
         <v>79818</v>
       </c>
-      <c r="E25" s="17">
+      <c r="E25" s="10">
         <v>42849</v>
       </c>
-      <c r="F25" s="17">
+      <c r="F25" s="10">
         <v>14319</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="17">
+      <c r="B26" s="10">
         <v>77933</v>
       </c>
-      <c r="C26" s="17">
+      <c r="C26" s="10">
         <v>71780</v>
       </c>
-      <c r="D26" s="17">
+      <c r="D26" s="10">
         <v>50172</v>
       </c>
-      <c r="E26" s="17">
+      <c r="E26" s="10">
         <v>28500</v>
       </c>
-      <c r="F26" s="17">
+      <c r="F26" s="10">
         <v>6152</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B27" s="17">
+      <c r="B27" s="10">
         <v>39563</v>
       </c>
-      <c r="C27" s="17">
+      <c r="C27" s="10">
         <v>34095</v>
       </c>
-      <c r="D27" s="17">
+      <c r="D27" s="10">
         <v>9535</v>
       </c>
-      <c r="E27" s="17">
+      <c r="E27" s="10">
         <v>28260</v>
       </c>
-      <c r="F27" s="17">
+      <c r="F27" s="10">
         <v>5468</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="17">
+      <c r="B28" s="10">
         <v>52295</v>
       </c>
-      <c r="C28" s="17">
+      <c r="C28" s="10">
         <v>45818</v>
       </c>
-      <c r="D28" s="17">
+      <c r="D28" s="10">
         <v>22357</v>
       </c>
-      <c r="E28" s="17">
+      <c r="E28" s="10">
         <v>30142</v>
       </c>
-      <c r="F28" s="17">
+      <c r="F28" s="10">
         <v>6478</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="17">
+      <c r="B29" s="10">
         <v>51792</v>
       </c>
-      <c r="C29" s="17">
+      <c r="C29" s="10">
         <v>46286</v>
       </c>
-      <c r="D29" s="17">
+      <c r="D29" s="10">
         <v>31043</v>
       </c>
-      <c r="E29" s="17">
+      <c r="E29" s="10">
         <v>21339</v>
       </c>
-      <c r="F29" s="17">
+      <c r="F29" s="10">
         <v>5506</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="17">
+      <c r="B30" s="10">
         <v>41533</v>
       </c>
-      <c r="C30" s="17">
+      <c r="C30" s="10">
         <v>37951</v>
       </c>
-      <c r="D30" s="17">
+      <c r="D30" s="10">
         <v>30128</v>
       </c>
-      <c r="E30" s="17">
+      <c r="E30" s="10">
         <v>12424</v>
       </c>
-      <c r="F30" s="17">
+      <c r="F30" s="10">
         <v>3581</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="17">
+      <c r="B31" s="10">
         <v>35351</v>
       </c>
-      <c r="C31" s="17">
+      <c r="C31" s="10">
         <v>33199</v>
       </c>
-      <c r="D31" s="17">
+      <c r="D31" s="10">
         <v>28229</v>
       </c>
-      <c r="E31" s="17">
+      <c r="E31" s="10">
         <v>8167</v>
       </c>
-      <c r="F31" s="17">
+      <c r="F31" s="10">
         <v>2153</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="17">
+      <c r="B32" s="10">
         <v>25262</v>
       </c>
-      <c r="C32" s="17">
+      <c r="C32" s="10">
         <v>23996</v>
       </c>
-      <c r="D32" s="17">
+      <c r="D32" s="10">
         <v>21131</v>
       </c>
-      <c r="E32" s="17">
+      <c r="E32" s="10">
         <v>5205</v>
       </c>
-      <c r="F32" s="17">
+      <c r="F32" s="10">
         <v>1266</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="17">
+      <c r="B33" s="10">
         <v>82278</v>
       </c>
-      <c r="C33" s="17">
+      <c r="C33" s="10">
         <v>79542</v>
       </c>
-      <c r="D33" s="17">
+      <c r="D33" s="10">
         <v>73942</v>
       </c>
-      <c r="E33" s="17">
+      <c r="E33" s="10">
         <v>11557</v>
       </c>
-      <c r="F33" s="17">
+      <c r="F33" s="10">
         <v>2735</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B34" s="17">
+      <c r="B34" s="10">
         <v>212530</v>
       </c>
-      <c r="C34" s="17">
+      <c r="C34" s="10">
         <v>188864</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D34" s="10">
         <v>152738</v>
       </c>
-      <c r="E34" s="17">
+      <c r="E34" s="10">
         <v>42305</v>
       </c>
-      <c r="F34" s="17">
+      <c r="F34" s="10">
         <v>23667</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="17">
+      <c r="B35" s="10">
         <v>155775</v>
       </c>
-      <c r="C35" s="17">
+      <c r="C35" s="10">
         <v>139347</v>
       </c>
-      <c r="D35" s="17">
+      <c r="D35" s="10">
         <v>124170</v>
       </c>
-      <c r="E35" s="17">
+      <c r="E35" s="10">
         <v>18913</v>
       </c>
-      <c r="F35" s="17">
+      <c r="F35" s="10">
         <v>16428</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="B36" s="17">
+      <c r="B36" s="10">
         <v>111015</v>
       </c>
-      <c r="C36" s="17">
+      <c r="C36" s="10">
         <v>100936</v>
       </c>
-      <c r="D36" s="17">
+      <c r="D36" s="10">
         <v>94415</v>
       </c>
-      <c r="E36" s="17">
+      <c r="E36" s="10">
         <v>8798</v>
       </c>
-      <c r="F36" s="17">
+      <c r="F36" s="10">
         <v>10079</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="B37" s="17">
+      <c r="B37" s="10">
         <v>44760</v>
       </c>
-      <c r="C37" s="17">
+      <c r="C37" s="10">
         <v>38412</v>
       </c>
-      <c r="D37" s="17">
+      <c r="D37" s="10">
         <v>29755</v>
       </c>
-      <c r="E37" s="17">
+      <c r="E37" s="10">
         <v>10116</v>
       </c>
-      <c r="F37" s="17">
+      <c r="F37" s="10">
         <v>6348</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B38" s="17">
+      <c r="B38" s="10">
         <v>56756</v>
       </c>
-      <c r="C38" s="17">
+      <c r="C38" s="10">
         <v>49517</v>
       </c>
-      <c r="D38" s="17">
+      <c r="D38" s="10">
         <v>28568</v>
       </c>
-      <c r="E38" s="17">
+      <c r="E38" s="10">
         <v>23392</v>
       </c>
-      <c r="F38" s="17">
+      <c r="F38" s="10">
         <v>7239</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A39" s="15" t="s">
+      <c r="A39" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B39" s="17">
+      <c r="B39" s="10">
         <v>212530</v>
       </c>
-      <c r="C39" s="17">
+      <c r="C39" s="10">
         <v>188864</v>
       </c>
-      <c r="D39" s="17">
+      <c r="D39" s="10">
         <v>152738</v>
       </c>
-      <c r="E39" s="17">
+      <c r="E39" s="10">
         <v>42305</v>
       </c>
-      <c r="F39" s="17">
+      <c r="F39" s="10">
         <v>23667</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B40" s="17">
+      <c r="B40" s="10">
         <v>16780</v>
       </c>
-      <c r="C40" s="17">
+      <c r="C40" s="10">
         <v>15359</v>
       </c>
-      <c r="D40" s="17">
+      <c r="D40" s="10">
         <v>7766</v>
       </c>
-      <c r="E40" s="17">
+      <c r="E40" s="10">
         <v>8774</v>
       </c>
-      <c r="F40" s="17">
+      <c r="F40" s="10">
         <v>1420</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="14" t="s">
+      <c r="A41" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B41" s="17">
+      <c r="B41" s="10">
         <v>194836</v>
       </c>
-      <c r="C41" s="17">
+      <c r="C41" s="10">
         <v>172593</v>
       </c>
-      <c r="D41" s="17">
+      <c r="D41" s="10">
         <v>144060</v>
       </c>
-      <c r="E41" s="17">
+      <c r="E41" s="10">
         <v>33485</v>
       </c>
-      <c r="F41" s="17">
+      <c r="F41" s="10">
         <v>22243</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A42" s="15" t="s">
+      <c r="A42" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="B42" s="17">
+      <c r="B42" s="10">
         <v>165810</v>
       </c>
-      <c r="C42" s="17">
+      <c r="C42" s="10">
         <v>147482</v>
       </c>
-      <c r="D42" s="17">
+      <c r="D42" s="10">
         <v>121532</v>
       </c>
-      <c r="E42" s="17">
+      <c r="E42" s="10">
         <v>30900</v>
       </c>
-      <c r="F42" s="17">
+      <c r="F42" s="10">
         <v>18328</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A43" s="14" t="s">
+      <c r="A43" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B43" s="17">
+      <c r="B43" s="10">
         <v>13604</v>
       </c>
-      <c r="C43" s="17">
+      <c r="C43" s="10">
         <v>9491</v>
       </c>
-      <c r="D43" s="17">
+      <c r="D43" s="10">
         <v>4664</v>
       </c>
-      <c r="E43" s="17">
+      <c r="E43" s="10">
         <v>5222</v>
       </c>
-      <c r="F43" s="17">
+      <c r="F43" s="10">
         <v>4114</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="49" x14ac:dyDescent="0.2">
-      <c r="A44" s="14" t="s">
+      <c r="A44" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B44" s="17">
+      <c r="B44" s="10">
         <v>45600</v>
       </c>
-      <c r="C44" s="17">
+      <c r="C44" s="10">
         <v>38437</v>
       </c>
-      <c r="D44" s="17">
+      <c r="D44" s="10">
         <v>27996</v>
       </c>
-      <c r="E44" s="17">
+      <c r="E44" s="10">
         <v>12035</v>
       </c>
-      <c r="F44" s="17">
+      <c r="F44" s="10">
         <v>7163</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A45" s="14" t="s">
+      <c r="A45" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="17">
+      <c r="B45" s="10">
         <v>23509</v>
       </c>
-      <c r="C45" s="17">
+      <c r="C45" s="10">
         <v>21003</v>
       </c>
-      <c r="D45" s="17">
+      <c r="D45" s="10">
         <v>16773</v>
       </c>
-      <c r="E45" s="17">
+      <c r="E45" s="10">
         <v>5194</v>
       </c>
-      <c r="F45" s="17">
+      <c r="F45" s="10">
         <v>2506</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A46" s="14" t="s">
+      <c r="A46" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B46" s="17">
+      <c r="B46" s="10">
         <v>17729</v>
       </c>
-      <c r="C46" s="17">
+      <c r="C46" s="10">
         <v>16233</v>
       </c>
-      <c r="D46" s="17">
+      <c r="D46" s="10">
         <v>13681</v>
       </c>
-      <c r="E46" s="17">
+      <c r="E46" s="10">
         <v>3197</v>
       </c>
-      <c r="F46" s="17">
+      <c r="F46" s="10">
         <v>1496</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A47" s="14" t="s">
+      <c r="A47" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B47" s="17">
+      <c r="B47" s="10">
         <v>41218</v>
       </c>
-      <c r="C47" s="17">
+      <c r="C47" s="10">
         <v>38974</v>
       </c>
-      <c r="D47" s="17">
+      <c r="D47" s="10">
         <v>36157</v>
       </c>
-      <c r="E47" s="17">
+      <c r="E47" s="10">
         <v>3691</v>
       </c>
-      <c r="F47" s="17">
+      <c r="F47" s="10">
         <v>2244</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A48" s="14" t="s">
+      <c r="A48" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B48" s="17">
+      <c r="B48" s="10">
         <v>24150</v>
       </c>
-      <c r="C48" s="17">
+      <c r="C48" s="10">
         <v>23345</v>
       </c>
-      <c r="D48" s="17">
+      <c r="D48" s="10">
         <v>22261</v>
       </c>
-      <c r="E48" s="17">
+      <c r="E48" s="10">
         <v>1561</v>
       </c>
-      <c r="F48" s="17">
+      <c r="F48" s="10">
         <v>805</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A49" s="15" t="s">
+      <c r="A49" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B49" s="17">
+      <c r="B49" s="10">
         <v>155775</v>
       </c>
-      <c r="C49" s="17">
+      <c r="C49" s="10">
         <v>139347</v>
       </c>
-      <c r="D49" s="17">
+      <c r="D49" s="10">
         <v>124170</v>
       </c>
-      <c r="E49" s="17">
+      <c r="E49" s="10">
         <v>18913</v>
       </c>
-      <c r="F49" s="17">
+      <c r="F49" s="10">
         <v>16428</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A50" s="14" t="s">
+      <c r="A50" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B50" s="17">
+      <c r="B50" s="10">
         <v>49215</v>
       </c>
-      <c r="C50" s="17">
+      <c r="C50" s="10">
         <v>40019</v>
       </c>
-      <c r="D50" s="17">
+      <c r="D50" s="10">
         <v>33047</v>
       </c>
-      <c r="E50" s="17">
+      <c r="E50" s="10">
         <v>8087</v>
       </c>
-      <c r="F50" s="17">
+      <c r="F50" s="10">
         <v>9196</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A51" s="14" t="s">
+      <c r="A51" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B51" s="17">
+      <c r="B51" s="10">
         <v>10460</v>
       </c>
-      <c r="C51" s="17">
+      <c r="C51" s="10">
         <v>9228</v>
       </c>
-      <c r="D51" s="17">
+      <c r="D51" s="10">
         <v>8158</v>
       </c>
-      <c r="E51" s="17">
+      <c r="E51" s="10">
         <v>1344</v>
       </c>
-      <c r="F51" s="17">
+      <c r="F51" s="10">
         <v>1231</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A52" s="14" t="s">
+      <c r="A52" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B52" s="17">
+      <c r="B52" s="10">
         <v>17955</v>
       </c>
-      <c r="C52" s="17">
+      <c r="C52" s="10">
         <v>16717</v>
       </c>
-      <c r="D52" s="17">
+      <c r="D52" s="10">
         <v>15419</v>
       </c>
-      <c r="E52" s="17">
+      <c r="E52" s="10">
         <v>1734</v>
       </c>
-      <c r="F52" s="17">
+      <c r="F52" s="10">
         <v>1238</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A53" s="14" t="s">
+      <c r="A53" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B53" s="17">
+      <c r="B53" s="10">
         <v>8048</v>
       </c>
-      <c r="C53" s="17">
+      <c r="C53" s="10">
         <v>7515</v>
       </c>
-      <c r="D53" s="17">
+      <c r="D53" s="10">
         <v>7049</v>
       </c>
-      <c r="E53" s="17">
+      <c r="E53" s="10">
         <v>645</v>
       </c>
-      <c r="F53" s="17">
+      <c r="F53" s="10">
         <v>533</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A54" s="14" t="s">
+      <c r="A54" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B54" s="17">
+      <c r="B54" s="10">
         <v>70096</v>
       </c>
-      <c r="C54" s="17">
+      <c r="C54" s="10">
         <v>65868</v>
       </c>
-      <c r="D54" s="17">
+      <c r="D54" s="10">
         <v>60496</v>
       </c>
-      <c r="E54" s="17">
+      <c r="E54" s="10">
         <v>7103</v>
       </c>
-      <c r="F54" s="17">
+      <c r="F54" s="10">
         <v>4229</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A55" s="15" t="s">
+      <c r="A55" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="B55" s="17">
+      <c r="B55" s="10">
         <v>327548</v>
       </c>
-      <c r="C55" s="17">
+      <c r="C55" s="10">
         <v>300418</v>
       </c>
-      <c r="D55" s="17">
+      <c r="D55" s="10">
         <v>216248</v>
       </c>
-      <c r="E55" s="17">
+      <c r="E55" s="10">
         <v>116697</v>
       </c>
-      <c r="F55" s="17">
+      <c r="F55" s="10">
         <v>27130</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A56" s="14" t="s">
+      <c r="A56" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B56" s="17">
+      <c r="B56" s="10">
         <v>37808</v>
       </c>
-      <c r="C56" s="17">
+      <c r="C56" s="10">
         <v>31697</v>
       </c>
-      <c r="D56" s="17">
+      <c r="D56" s="10">
         <v>8552</v>
       </c>
-      <c r="E56" s="17">
+      <c r="E56" s="10">
         <v>25225</v>
       </c>
-      <c r="F56" s="17">
+      <c r="F56" s="10">
         <v>6111</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A57" s="14" t="s">
+      <c r="A57" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B57" s="17">
+      <c r="B57" s="10">
         <v>56839</v>
       </c>
-      <c r="C57" s="17">
+      <c r="C57" s="10">
         <v>47917</v>
       </c>
-      <c r="D57" s="17">
+      <c r="D57" s="10">
         <v>13606</v>
       </c>
-      <c r="E57" s="17">
+      <c r="E57" s="10">
         <v>37750</v>
       </c>
-      <c r="F57" s="17">
+      <c r="F57" s="10">
         <v>8922</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="37" x14ac:dyDescent="0.2">
-      <c r="A58" s="14" t="s">
+      <c r="A58" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B58" s="17">
+      <c r="B58" s="10">
         <v>52533</v>
       </c>
-      <c r="C58" s="17">
+      <c r="C58" s="10">
         <v>45595</v>
       </c>
-      <c r="D58" s="17">
+      <c r="D58" s="10">
         <v>20276</v>
       </c>
-      <c r="E58" s="17">
+      <c r="E58" s="10">
         <v>30161</v>
       </c>
-      <c r="F58" s="17">
+      <c r="F58" s="10">
         <v>6938</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="37" x14ac:dyDescent="0.2">
-      <c r="A59" s="14" t="s">
+      <c r="A59" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B59" s="17">
+      <c r="B59" s="10">
         <v>49916</v>
       </c>
-      <c r="C59" s="17">
+      <c r="C59" s="10">
         <v>44438</v>
       </c>
-      <c r="D59" s="17">
+      <c r="D59" s="10">
         <v>29988</v>
       </c>
-      <c r="E59" s="17">
+      <c r="E59" s="10">
         <v>19625</v>
       </c>
-      <c r="F59" s="17">
+      <c r="F59" s="10">
         <v>5478</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="37" x14ac:dyDescent="0.2">
-      <c r="A60" s="14" t="s">
+      <c r="A60" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B60" s="17">
+      <c r="B60" s="10">
         <v>42688</v>
       </c>
-      <c r="C60" s="17">
+      <c r="C60" s="10">
         <v>38888</v>
       </c>
-      <c r="D60" s="17">
+      <c r="D60" s="10">
         <v>30360</v>
       </c>
-      <c r="E60" s="17">
+      <c r="E60" s="10">
         <v>13142</v>
       </c>
-      <c r="F60" s="17">
+      <c r="F60" s="10">
         <v>3799</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A61" s="14" t="s">
+      <c r="A61" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B61" s="17">
+      <c r="B61" s="10">
         <v>144603</v>
       </c>
-      <c r="C61" s="17">
+      <c r="C61" s="10">
         <v>139799</v>
       </c>
-      <c r="D61" s="17">
+      <c r="D61" s="10">
         <v>127072</v>
       </c>
-      <c r="E61" s="17">
+      <c r="E61" s="10">
         <v>28545</v>
       </c>
-      <c r="F61" s="17">
+      <c r="F61" s="10">
         <v>4804</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="14" t="s">
+      <c r="A62" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B62" s="17">
+      <c r="B62" s="10">
         <v>98070</v>
       </c>
-      <c r="C62" s="17">
+      <c r="C62" s="10">
         <v>91120</v>
       </c>
-      <c r="D62" s="17">
+      <c r="D62" s="10">
         <v>73692</v>
       </c>
-      <c r="E62" s="17">
+      <c r="E62" s="10">
         <v>22431</v>
       </c>
-      <c r="F62" s="17">
+      <c r="F62" s="10">
         <v>6950</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="14" t="s">
+      <c r="A63" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B63" s="17">
+      <c r="B63" s="10">
         <v>107795</v>
       </c>
-      <c r="C63" s="17">
+      <c r="C63" s="10">
         <v>99068</v>
       </c>
-      <c r="D63" s="17">
+      <c r="D63" s="10">
         <v>77499</v>
       </c>
-      <c r="E63" s="17">
+      <c r="E63" s="10">
         <v>31904</v>
       </c>
-      <c r="F63" s="17">
+      <c r="F63" s="10">
         <v>8727</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="14" t="s">
+      <c r="A64" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B64" s="17">
+      <c r="B64" s="10">
         <v>85448</v>
       </c>
-      <c r="C64" s="17">
+      <c r="C64" s="10">
         <v>76704</v>
       </c>
-      <c r="D64" s="17">
+      <c r="D64" s="10">
         <v>50558</v>
       </c>
-      <c r="E64" s="17">
+      <c r="E64" s="10">
         <v>37321</v>
       </c>
-      <c r="F64" s="17">
+      <c r="F64" s="10">
         <v>8744</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="14" t="s">
+      <c r="A65" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B65" s="17">
+      <c r="B65" s="10">
         <v>36762</v>
       </c>
-      <c r="C65" s="17">
+      <c r="C65" s="10">
         <v>33996</v>
       </c>
-      <c r="D65" s="17">
+      <c r="D65" s="10">
         <v>14618</v>
       </c>
-      <c r="E65" s="17">
+      <c r="E65" s="10">
         <v>25438</v>
       </c>
-      <c r="F65" s="17">
+      <c r="F65" s="10">
         <v>2766</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A66" s="15" t="s">
+      <c r="A66" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B66" s="17">
+      <c r="B66" s="10">
         <v>194855</v>
       </c>
-      <c r="C66" s="17">
+      <c r="C66" s="10">
         <v>172209</v>
       </c>
-      <c r="D66" s="17">
+      <c r="D66" s="10">
         <v>141344</v>
       </c>
-      <c r="E66" s="17">
+      <c r="E66" s="10">
         <v>36483</v>
       </c>
-      <c r="F66" s="17">
+      <c r="F66" s="10">
         <v>22646</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="14" t="s">
+      <c r="A67" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B67" s="17">
+      <c r="B67" s="10">
         <v>99078</v>
       </c>
-      <c r="C67" s="17">
+      <c r="C67" s="10">
         <v>91013</v>
       </c>
-      <c r="D67" s="17">
+      <c r="D67" s="10">
         <v>80941</v>
       </c>
-      <c r="E67" s="17">
+      <c r="E67" s="10">
         <v>13306</v>
       </c>
-      <c r="F67" s="17">
+      <c r="F67" s="10">
         <v>8065</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="14" t="s">
+      <c r="A68" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B68" s="17">
+      <c r="B68" s="10">
         <v>3267</v>
       </c>
-      <c r="C68" s="17">
+      <c r="C68" s="10">
         <v>2865</v>
       </c>
-      <c r="D68" s="17">
+      <c r="D68" s="10">
         <v>1816</v>
       </c>
-      <c r="E68" s="17">
+      <c r="E68" s="10">
         <v>1180</v>
       </c>
-      <c r="F68" s="17">
+      <c r="F68" s="10">
         <v>402</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="14" t="s">
+      <c r="A69" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B69" s="17">
+      <c r="B69" s="10">
         <v>18138</v>
       </c>
-      <c r="C69" s="17">
+      <c r="C69" s="10">
         <v>15865</v>
       </c>
-      <c r="D69" s="17">
+      <c r="D69" s="10">
         <v>11694</v>
       </c>
-      <c r="E69" s="17">
+      <c r="E69" s="10">
         <v>4688</v>
       </c>
-      <c r="F69" s="17">
+      <c r="F69" s="10">
         <v>2273</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="14" t="s">
+      <c r="A70" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B70" s="17">
+      <c r="B70" s="10">
         <v>3898</v>
       </c>
-      <c r="C70" s="17">
+      <c r="C70" s="10">
         <v>3158</v>
       </c>
-      <c r="D70" s="17">
+      <c r="D70" s="10">
         <v>2147</v>
       </c>
-      <c r="E70" s="17">
+      <c r="E70" s="10">
         <v>1134</v>
       </c>
-      <c r="F70" s="17">
+      <c r="F70" s="10">
         <v>739</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="14" t="s">
+      <c r="A71" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B71" s="17">
+      <c r="B71" s="10">
         <v>70474</v>
       </c>
-      <c r="C71" s="17">
+      <c r="C71" s="10">
         <v>59307</v>
       </c>
-      <c r="D71" s="17">
+      <c r="D71" s="10">
         <v>44746</v>
       </c>
-      <c r="E71" s="17">
+      <c r="E71" s="10">
         <v>16175</v>
       </c>
-      <c r="F71" s="17">
+      <c r="F71" s="10">
         <v>11166</v>
       </c>
     </row>
@@ -7726,233 +7758,251 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8A5DE9C-C28D-3E40-B561-4B209DF88386}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="176" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="52" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:6" ht="28" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>122</v>
+      <c r="B1" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="10">
         <v>13604</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="10">
         <v>9491</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="10">
         <v>4664</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="10">
         <v>5222</v>
       </c>
-      <c r="F2" s="17">
+      <c r="F2" s="10">
         <v>4114</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="49" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="10">
         <v>45600</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="10">
         <v>38437</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="10">
         <v>27996</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="10">
         <v>12035</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="10">
         <v>7163</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="10">
         <v>23509</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="10">
         <v>21003</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="10">
         <v>16773</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="10">
         <v>5194</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="10">
         <v>2506</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="10">
         <v>17729</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="10">
         <v>16233</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="10">
         <v>13681</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="10">
         <v>3197</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="10">
         <v>1496</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="10">
         <v>41218</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="10">
         <v>38974</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="10">
         <v>36157</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="10">
         <v>3691</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="10">
         <v>2244</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="10">
         <v>24150</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="10">
         <v>23345</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="10">
         <v>22261</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="10">
         <v>1561</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="10">
         <v>805</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="10">
         <v>281229</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="10">
         <v>263172</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="10">
         <v>190775</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="10">
         <v>102229</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="10">
         <v>18057</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="10">
         <v>46845</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="10">
         <v>37715</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="10">
         <v>25591</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="10">
         <v>14865</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="10">
         <v>9130</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="25" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="10">
         <v>22877</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="10">
         <v>21078</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="10">
         <v>14301</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="10">
         <v>8863</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="10">
         <v>1799</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="10">
         <v>23968</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="10">
         <v>16637</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="10">
         <v>11290</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="10">
         <v>6003</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="10">
         <v>7331</v>
       </c>
+    </row>
+    <row r="18" spans="6:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F18" s="18"/>
+    </row>
+    <row r="19" spans="6:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F19" s="18"/>
+    </row>
+    <row r="20" spans="6:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F20" s="18"/>
+    </row>
+    <row r="21" spans="6:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F21" s="18"/>
+    </row>
+    <row r="22" spans="6:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F22" s="18"/>
+    </row>
+    <row r="23" spans="6:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F23" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>